<commit_message>
Add gainain to canvas
</commit_message>
<xml_diff>
--- a/交易复盘记录20220201.xlsx
+++ b/交易复盘记录20220201.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gao'guang\Desktop\Atool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A187F9AC-00A3-41FB-85AE-BD08C69EECFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DBF766-C729-4130-B464-E8D229EED3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="交易模式" sheetId="1" r:id="rId1"/>
-    <sheet name="新能源" sheetId="19" r:id="rId2"/>
-    <sheet name="情绪" sheetId="11" r:id="rId3"/>
-    <sheet name="0706" sheetId="25" r:id="rId4"/>
-    <sheet name="0705" sheetId="23" r:id="rId5"/>
-    <sheet name="0704" sheetId="2" r:id="rId6"/>
-    <sheet name="0701" sheetId="22" state="hidden" r:id="rId7"/>
-    <sheet name="周期" sheetId="14" r:id="rId8"/>
+    <sheet name="交易模式" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="周期" sheetId="14" state="hidden" r:id="rId2"/>
+    <sheet name="新能源" sheetId="19" state="hidden" r:id="rId3"/>
+    <sheet name="情绪" sheetId="11" r:id="rId4"/>
+    <sheet name="0706" sheetId="25" r:id="rId5"/>
+    <sheet name="0705" sheetId="23" r:id="rId6"/>
+    <sheet name="0704" sheetId="2" r:id="rId7"/>
+    <sheet name="个股" sheetId="22" state="hidden" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="702">
   <si>
     <t>板块</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2613,6 +2613,18 @@
   </si>
   <si>
     <t>医药+新冠治疗</t>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抽水蓄能+光伏+电力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>家电+新股</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3111,32 +3123,32 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3147,19 +3159,19 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4107,6 +4119,678 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E0BFF9-F567-4705-9C7E-E21C99F47D06}">
+  <dimension ref="A1:T50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.35546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>2020</v>
+      </c>
+      <c r="B1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="22">
+        <v>44877</v>
+      </c>
+      <c r="D1" s="85" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C2" s="22">
+        <v>44923</v>
+      </c>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2021</v>
+      </c>
+      <c r="B3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="22">
+        <v>44566</v>
+      </c>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>3500</v>
+      </c>
+      <c r="C4" s="22">
+        <v>44574</v>
+      </c>
+      <c r="D4" s="88" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="85"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C5" s="23">
+        <v>44580</v>
+      </c>
+      <c r="D5" s="88"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C6" s="23">
+        <v>44596</v>
+      </c>
+      <c r="E6" s="88" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C7" s="23">
+        <v>44600</v>
+      </c>
+      <c r="E7" s="88"/>
+      <c r="F7" s="83" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>3700</v>
+      </c>
+      <c r="C8" s="23">
+        <v>44616</v>
+      </c>
+      <c r="E8" s="88"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C9" s="23">
+        <v>44628</v>
+      </c>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>3300</v>
+      </c>
+      <c r="C10" s="23">
+        <v>44632</v>
+      </c>
+      <c r="G10" s="86" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C11" s="22">
+        <v>44657</v>
+      </c>
+      <c r="D11" s="87" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" s="86"/>
+      <c r="H11" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="I11" s="83" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C12" s="22">
+        <v>44678</v>
+      </c>
+      <c r="D12" s="87"/>
+      <c r="E12" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="F12" s="81" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" s="80"/>
+      <c r="I12" s="83"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C13" s="22">
+        <v>44700</v>
+      </c>
+      <c r="D13" s="87"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="82" t="s">
+        <v>106</v>
+      </c>
+      <c r="H13" s="80"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="83" t="s">
+        <v>104</v>
+      </c>
+      <c r="K13" s="84" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C14" s="22"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="83"/>
+      <c r="J14" s="83"/>
+      <c r="K14" s="84"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B15">
+        <v>3600</v>
+      </c>
+      <c r="C15" s="22">
+        <v>44720</v>
+      </c>
+      <c r="E15" s="80"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="80"/>
+      <c r="J15" s="83"/>
+      <c r="K15" s="84"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C16" s="22">
+        <v>44729</v>
+      </c>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="82"/>
+      <c r="H16" s="80"/>
+      <c r="J16" s="83"/>
+      <c r="K16" s="84"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C17" s="22">
+        <v>44736</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="H17" s="80"/>
+      <c r="K17" s="82" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C18" s="22">
+        <v>44743</v>
+      </c>
+      <c r="G18" s="81" t="s">
+        <v>107</v>
+      </c>
+      <c r="H18" s="80"/>
+      <c r="I18" s="80" t="s">
+        <v>108</v>
+      </c>
+      <c r="J18" s="81" t="s">
+        <v>109</v>
+      </c>
+      <c r="K18" s="82"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>3300</v>
+      </c>
+      <c r="G19" s="81"/>
+      <c r="I19" s="80"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="82"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C20" s="22">
+        <v>44779</v>
+      </c>
+      <c r="G20" s="81"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="82"/>
+      <c r="L20" s="80" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C21" s="22"/>
+      <c r="G21" s="81"/>
+      <c r="I21" s="80"/>
+      <c r="J21" s="81"/>
+      <c r="K21" s="82"/>
+      <c r="L21" s="80"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C22" s="22">
+        <v>44805</v>
+      </c>
+      <c r="G22" s="81"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="81"/>
+      <c r="K22" s="82"/>
+      <c r="L22" s="80"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <v>3700</v>
+      </c>
+      <c r="C23" s="22">
+        <v>44818</v>
+      </c>
+      <c r="G23" s="81"/>
+      <c r="K23" s="82"/>
+      <c r="L23" s="80"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L24" s="80"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C25" s="22">
+        <v>44863</v>
+      </c>
+      <c r="L25" s="80"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C26" s="22">
+        <v>44866</v>
+      </c>
+      <c r="L26" s="80"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C27" s="22">
+        <v>44884</v>
+      </c>
+      <c r="K27" s="83" t="s">
+        <v>112</v>
+      </c>
+      <c r="L27" s="83" t="s">
+        <v>113</v>
+      </c>
+      <c r="M27" s="84" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>2022</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="22">
+        <v>44916</v>
+      </c>
+      <c r="K28" s="83"/>
+      <c r="L28" s="83"/>
+      <c r="M28" s="84"/>
+      <c r="N28" s="83" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B29">
+        <v>3700</v>
+      </c>
+      <c r="C29" s="22">
+        <v>1</v>
+      </c>
+      <c r="L29" s="83"/>
+      <c r="N29" s="83"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C30" s="22">
+        <v>44579</v>
+      </c>
+      <c r="L30" s="83"/>
+      <c r="N30" s="83"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C31" s="22">
+        <v>44599</v>
+      </c>
+      <c r="M31" s="83" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>173</v>
+      </c>
+      <c r="B32" t="s">
+        <v>177</v>
+      </c>
+      <c r="C32" s="22">
+        <v>44622</v>
+      </c>
+      <c r="K32" s="90" t="s">
+        <v>167</v>
+      </c>
+      <c r="M32" s="83"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C33" s="22">
+        <v>44631</v>
+      </c>
+      <c r="K33" s="91"/>
+      <c r="M33" s="83"/>
+      <c r="N33" s="90" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C34" s="22">
+        <v>44641</v>
+      </c>
+      <c r="K34" s="91"/>
+      <c r="M34" s="83"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="83" t="s">
+        <v>116</v>
+      </c>
+      <c r="T34" s="92" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>174</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="22">
+        <v>44663</v>
+      </c>
+      <c r="N35" s="91"/>
+      <c r="O35" s="83"/>
+      <c r="T35" s="92"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <v>2860</v>
+      </c>
+      <c r="C36" s="22">
+        <v>44676</v>
+      </c>
+      <c r="K36" s="83" t="s">
+        <v>119</v>
+      </c>
+      <c r="L36" s="89" t="s">
+        <v>172</v>
+      </c>
+      <c r="M36" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="N36" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="O36" s="83"/>
+      <c r="T36" s="92"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C37" s="22">
+        <v>44694</v>
+      </c>
+      <c r="I37" s="92" t="s">
+        <v>123</v>
+      </c>
+      <c r="J37" s="93" t="s">
+        <v>170</v>
+      </c>
+      <c r="K37" s="83"/>
+      <c r="L37" s="84"/>
+      <c r="M37" s="83"/>
+      <c r="N37" s="83"/>
+      <c r="O37" s="83"/>
+      <c r="P37" s="84" t="s">
+        <v>168</v>
+      </c>
+      <c r="R37" s="94" t="s">
+        <v>166</v>
+      </c>
+      <c r="S37" s="83" t="s">
+        <v>120</v>
+      </c>
+      <c r="T37" s="92"/>
+    </row>
+    <row r="38" spans="1:20" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>175</v>
+      </c>
+      <c r="B38" t="s">
+        <v>178</v>
+      </c>
+      <c r="C38" s="22">
+        <v>44702</v>
+      </c>
+      <c r="D38" s="85" t="s">
+        <v>122</v>
+      </c>
+      <c r="I38" s="92"/>
+      <c r="J38" s="85"/>
+      <c r="K38" s="83"/>
+      <c r="L38" s="83" t="s">
+        <v>118</v>
+      </c>
+      <c r="M38" s="83"/>
+      <c r="N38" s="83"/>
+      <c r="O38" s="84" t="s">
+        <v>121</v>
+      </c>
+      <c r="P38" s="84"/>
+      <c r="Q38" s="84" t="s">
+        <v>169</v>
+      </c>
+      <c r="R38" s="86"/>
+      <c r="S38" s="83"/>
+      <c r="T38" s="92"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C39" s="22">
+        <v>44721</v>
+      </c>
+      <c r="D39" s="85"/>
+      <c r="E39" s="92" t="s">
+        <v>145</v>
+      </c>
+      <c r="G39" s="84" t="s">
+        <v>124</v>
+      </c>
+      <c r="I39" s="92"/>
+      <c r="J39" s="85"/>
+      <c r="L39" s="83"/>
+      <c r="O39" s="84"/>
+      <c r="P39" s="84"/>
+      <c r="Q39" s="84"/>
+      <c r="R39" s="86"/>
+      <c r="S39" s="83"/>
+      <c r="T39" s="92"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C40" s="22">
+        <v>44725</v>
+      </c>
+      <c r="D40" s="85"/>
+      <c r="E40" s="92"/>
+      <c r="G40" s="84"/>
+      <c r="H40" s="83" t="s">
+        <v>73</v>
+      </c>
+      <c r="I40" s="92"/>
+      <c r="J40" s="85"/>
+      <c r="L40" s="33"/>
+      <c r="O40" s="84"/>
+      <c r="P40" s="34"/>
+      <c r="Q40" s="34"/>
+      <c r="R40" s="86"/>
+      <c r="S40" s="83"/>
+      <c r="T40" s="35"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A41" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="B41">
+        <v>3316</v>
+      </c>
+      <c r="C41" s="22">
+        <v>44729</v>
+      </c>
+      <c r="D41" s="85"/>
+      <c r="E41" s="92"/>
+      <c r="G41" s="84"/>
+      <c r="H41" s="83"/>
+      <c r="I41" s="92"/>
+      <c r="J41" s="85"/>
+      <c r="O41" s="84"/>
+      <c r="R41" s="86"/>
+      <c r="S41" s="83"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="D42" s="85"/>
+      <c r="E42" s="92"/>
+      <c r="G42" s="84"/>
+      <c r="H42" s="83"/>
+      <c r="I42" s="92"/>
+      <c r="J42" s="85"/>
+      <c r="O42" s="84"/>
+      <c r="R42" s="86"/>
+      <c r="S42" s="83"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A43" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="D43" s="85"/>
+      <c r="E43" s="92"/>
+      <c r="G43" s="84"/>
+      <c r="H43" s="83"/>
+      <c r="I43" s="92"/>
+      <c r="J43" s="85"/>
+      <c r="O43" s="84"/>
+      <c r="R43" s="86"/>
+      <c r="S43" s="83"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="D44" s="85"/>
+      <c r="E44" s="92"/>
+      <c r="G44" s="84"/>
+      <c r="H44" s="83"/>
+      <c r="I44" s="92"/>
+      <c r="J44" s="85"/>
+      <c r="O44" s="84"/>
+      <c r="R44" s="86"/>
+      <c r="S44" s="83"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="D45" s="85"/>
+      <c r="E45" s="92"/>
+      <c r="G45" s="84"/>
+      <c r="H45" s="83"/>
+      <c r="I45" s="92"/>
+      <c r="J45" s="85"/>
+      <c r="R45" s="86"/>
+      <c r="S45" s="83"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="D46" s="85"/>
+      <c r="E46" s="92"/>
+      <c r="G46" s="84"/>
+      <c r="H46" s="83"/>
+      <c r="I46" s="92"/>
+      <c r="J46" s="85"/>
+      <c r="R46" s="86"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="E47" s="92"/>
+      <c r="H47" s="83"/>
+      <c r="I47" s="92"/>
+      <c r="J47" s="85"/>
+      <c r="R47" s="86"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="E48" s="92"/>
+      <c r="H48" s="83"/>
+    </row>
+    <row r="49" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E49" s="92"/>
+      <c r="H49" s="83"/>
+    </row>
+    <row r="50" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E50" s="92"/>
+    </row>
+  </sheetData>
+  <mergeCells count="46">
+    <mergeCell ref="E39:E50"/>
+    <mergeCell ref="D38:D46"/>
+    <mergeCell ref="I37:I47"/>
+    <mergeCell ref="G39:G46"/>
+    <mergeCell ref="S37:S45"/>
+    <mergeCell ref="K36:K38"/>
+    <mergeCell ref="P37:P39"/>
+    <mergeCell ref="H40:H49"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="O38:O44"/>
+    <mergeCell ref="J37:J47"/>
+    <mergeCell ref="R37:R47"/>
+    <mergeCell ref="Q38:Q39"/>
+    <mergeCell ref="M36:M38"/>
+    <mergeCell ref="O34:O37"/>
+    <mergeCell ref="N36:N38"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="N33:N35"/>
+    <mergeCell ref="K32:K34"/>
+    <mergeCell ref="T34:T39"/>
+    <mergeCell ref="N28:N30"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G18:G23"/>
+    <mergeCell ref="G13:G16"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="L20:L26"/>
+    <mergeCell ref="M31:M34"/>
+    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="L27:L30"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="H11:H18"/>
+    <mergeCell ref="I18:I22"/>
+    <mergeCell ref="J18:J22"/>
+    <mergeCell ref="K17:K23"/>
+    <mergeCell ref="J13:J16"/>
+    <mergeCell ref="K13:K16"/>
+    <mergeCell ref="I11:I14"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2297A66E-7AB8-44E3-AC13-79B13077F72D}">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -4351,12 +5035,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7566D60B-D225-4CB7-8BAE-ACECC645510D}">
-  <dimension ref="A1:Q51"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4368,7 +5052,7 @@
     <col min="12" max="12" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>62</v>
       </c>
@@ -4396,16 +5080,8 @@
       <c r="I1" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="10">
         <v>44713</v>
       </c>
@@ -4434,16 +5110,8 @@
       <c r="I2" s="64">
         <v>3182</v>
       </c>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
         <v>44714</v>
       </c>
@@ -4473,16 +5141,8 @@
       <c r="I3" s="64">
         <v>3195</v>
       </c>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="78"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
         <v>44718</v>
       </c>
@@ -4512,16 +5172,8 @@
       <c r="I4" s="64">
         <v>3236</v>
       </c>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="78"/>
-      <c r="Q4" s="78"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="10">
         <v>44719</v>
       </c>
@@ -4551,16 +5203,8 @@
       <c r="I5" s="64">
         <v>3241</v>
       </c>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="78"/>
-      <c r="Q5" s="78"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="10">
         <v>44720</v>
       </c>
@@ -4590,16 +5234,8 @@
       <c r="I6" s="64">
         <v>3263</v>
       </c>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="78"/>
-      <c r="O6" s="78"/>
-      <c r="P6" s="78"/>
-      <c r="Q6" s="78"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="10">
         <v>44721</v>
       </c>
@@ -4629,16 +5265,8 @@
       <c r="I7" s="64">
         <v>3248</v>
       </c>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="78"/>
-      <c r="M7" s="78"/>
-      <c r="N7" s="78"/>
-      <c r="O7" s="78"/>
-      <c r="P7" s="78"/>
-      <c r="Q7" s="78"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="10">
         <v>44722</v>
       </c>
@@ -4668,16 +5296,8 @@
       <c r="I8" s="64">
         <v>3284</v>
       </c>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="78"/>
-      <c r="P8" s="78"/>
-      <c r="Q8" s="78"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="10">
         <v>44725</v>
       </c>
@@ -4707,16 +5327,8 @@
       <c r="I9" s="64">
         <v>3255</v>
       </c>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="78"/>
-      <c r="N9" s="78"/>
-      <c r="O9" s="78"/>
-      <c r="P9" s="78"/>
-      <c r="Q9" s="78"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="10">
         <v>44726</v>
       </c>
@@ -4746,16 +5358,8 @@
       <c r="I10" s="64">
         <v>3248</v>
       </c>
-      <c r="J10" s="78"/>
-      <c r="K10" s="78"/>
-      <c r="L10" s="78"/>
-      <c r="M10" s="78"/>
-      <c r="N10" s="78"/>
-      <c r="O10" s="78"/>
-      <c r="P10" s="78"/>
-      <c r="Q10" s="78"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>44727</v>
       </c>
@@ -4785,16 +5389,8 @@
       <c r="I11" s="1">
         <v>3305</v>
       </c>
-      <c r="J11" s="78"/>
-      <c r="K11" s="78"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="78"/>
-      <c r="N11" s="78"/>
-      <c r="O11" s="78"/>
-      <c r="P11" s="78"/>
-      <c r="Q11" s="78"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>44728</v>
       </c>
@@ -4828,7 +5424,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="19">
         <v>44729</v>
       </c>
@@ -4862,7 +5458,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="19">
         <v>44732</v>
       </c>
@@ -4896,7 +5492,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="19">
         <v>44733</v>
       </c>
@@ -4930,7 +5526,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="19">
         <v>44734</v>
       </c>
@@ -5389,79 +5985,17 @@
       <c r="I51" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="J1:Q4"/>
-    <mergeCell ref="J5:Q8"/>
-    <mergeCell ref="J9:Q11"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
-      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup dateAxis="1" displayEmptyCellsAs="gap" markers="1" high="1" low="1" first="1" last="1" negative="1" xr2:uid="{7A022841-4C66-4547-933A-63CE3C1373CA}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <xm:f>情绪!A2:A26</xm:f>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>情绪!I2:I51</xm:f>
-              <xm:sqref>J9</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup dateAxis="1" displayEmptyCellsAs="gap" markers="1" high="1" low="1" first="1" last="1" negative="1" xr2:uid="{87187A59-C3EE-4963-9125-5402CE55C0B7}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <xm:f>情绪!A2:A26</xm:f>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>情绪!H2:H51</xm:f>
-              <xm:sqref>J1</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" dateAxis="1" displayEmptyCellsAs="gap" markers="1" high="1" low="1" first="1" last="1" negative="1" xr2:uid="{9A5423CA-A8BE-450A-A1F0-3BE57C5E8F4E}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <xm:f>情绪!A2:A26</xm:f>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>情绪!E2:E51</xm:f>
-              <xm:sqref>J5</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-      </x14:sparklineGroups>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49393269-8524-41E4-AA15-EFA7F2F95046}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -5488,67 +6022,67 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>375</v>
+        <v>358</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>376</v>
+        <v>273</v>
       </c>
       <c r="C2" s="9">
-        <v>14366703000</v>
+        <v>11249532100</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>377</v>
+        <v>274</v>
       </c>
       <c r="E2" s="9">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>358</v>
+        <v>496</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="C3" s="9">
-        <v>11249532100</v>
+        <v>1094983690</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="E3" s="9">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>496</v>
+        <v>129</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>283</v>
+        <v>130</v>
       </c>
       <c r="C4" s="9">
-        <v>1094983690</v>
+        <v>12360768200</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="E4" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>129</v>
+        <v>497</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>130</v>
+        <v>298</v>
       </c>
       <c r="C5" s="9">
-        <v>12360768200</v>
+        <v>1017200000</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E5" s="9">
         <v>4</v>
@@ -5556,16 +6090,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>497</v>
+        <v>315</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C6" s="9">
-        <v>1017200000</v>
+        <v>47843132000</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="E6" s="9">
         <v>4</v>
@@ -5573,33 +6107,33 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>315</v>
+        <v>333</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>300</v>
+        <v>334</v>
       </c>
       <c r="C7" s="9">
-        <v>47843132000</v>
+        <v>2451663900</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>301</v>
+        <v>502</v>
       </c>
       <c r="E7" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="C8" s="9">
-        <v>2451663900</v>
+        <v>4732854300</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>502</v>
+        <v>588</v>
       </c>
       <c r="E8" s="9">
         <v>3</v>
@@ -5607,33 +6141,33 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>325</v>
+        <v>504</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>326</v>
+        <v>146</v>
       </c>
       <c r="C9" s="9">
-        <v>4732854300</v>
+        <v>2530192100</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>588</v>
+        <v>147</v>
       </c>
       <c r="E9" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>146</v>
+        <v>506</v>
       </c>
       <c r="C10" s="9">
-        <v>2530192100</v>
+        <v>3366800000</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>147</v>
+        <v>589</v>
       </c>
       <c r="E10" s="9">
         <v>2</v>
@@ -5641,16 +6175,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>505</v>
+        <v>529</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>506</v>
+        <v>530</v>
       </c>
       <c r="C11" s="9">
-        <v>3366800000</v>
+        <v>1529306600</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="E11" s="9">
         <v>2</v>
@@ -5658,16 +6192,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>529</v>
+        <v>576</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>530</v>
+        <v>577</v>
       </c>
       <c r="C12" s="9">
-        <v>1529306600</v>
+        <v>3071749300</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
       <c r="E12" s="9">
         <v>2</v>
@@ -5675,33 +6209,33 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>576</v>
+        <v>591</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>577</v>
+        <v>592</v>
       </c>
       <c r="C13" s="9">
-        <v>3071749300</v>
+        <v>1728310500</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>578</v>
+        <v>593</v>
       </c>
       <c r="E13" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="C14" s="9">
-        <v>1728310500</v>
+        <v>3281594100</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="E14" s="9">
         <v>1</v>
@@ -5709,16 +6243,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="C15" s="9">
-        <v>3281594100</v>
+        <v>1752310800</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="E15" s="9">
         <v>1</v>
@@ -5726,16 +6260,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="C16" s="9">
-        <v>1752310800</v>
+        <v>5616643400</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="E16" s="9">
         <v>1</v>
@@ -5743,16 +6277,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="C17" s="9">
-        <v>5616643400</v>
+        <v>1375305100</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="E17" s="9">
         <v>1</v>
@@ -5760,16 +6294,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="C18" s="9">
-        <v>1375305100</v>
+        <v>3736154000</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>605</v>
+        <v>127</v>
       </c>
       <c r="E18" s="9">
         <v>1</v>
@@ -5777,13 +6311,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="C19" s="9">
-        <v>3736154000</v>
+        <v>2805656700</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>127</v>
@@ -5794,16 +6328,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="C20" s="9">
-        <v>2805656700</v>
+        <v>4380056400</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>127</v>
+        <v>612</v>
       </c>
       <c r="E20" s="9">
         <v>1</v>
@@ -5811,16 +6345,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="C21" s="9">
-        <v>4380056400</v>
+        <v>3415350800</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="E21" s="9">
         <v>1</v>
@@ -5828,16 +6362,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="C22" s="9">
-        <v>3415350800</v>
+        <v>4908974900</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="E22" s="9">
         <v>1</v>
@@ -5845,16 +6379,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="C23" s="9">
-        <v>4908974900</v>
+        <v>3397208700</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="E23" s="9">
         <v>1</v>
@@ -5862,16 +6396,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>619</v>
+        <v>341</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>620</v>
+        <v>293</v>
       </c>
       <c r="C24" s="9">
-        <v>3397208700</v>
+        <v>2689697400</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>621</v>
+        <v>294</v>
       </c>
       <c r="E24" s="9">
         <v>1</v>
@@ -5879,16 +6413,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
-        <v>341</v>
+        <v>622</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>293</v>
+        <v>623</v>
       </c>
       <c r="C25" s="9">
-        <v>2689697400</v>
+        <v>3683356500</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>294</v>
+        <v>624</v>
       </c>
       <c r="E25" s="9">
         <v>1</v>
@@ -5896,16 +6430,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="C26" s="9">
-        <v>3683356500</v>
+        <v>3077923800</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="E26" s="9">
         <v>1</v>
@@ -5913,16 +6447,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>626</v>
+        <v>131</v>
       </c>
       <c r="C27" s="9">
-        <v>3077923800</v>
+        <v>7947959100</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="E27" s="9">
         <v>1</v>
@@ -5930,16 +6464,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>131</v>
+        <v>631</v>
       </c>
       <c r="C28" s="9">
-        <v>7947959100</v>
+        <v>8686938200</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="E28" s="9">
         <v>1</v>
@@ -5947,16 +6481,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="C29" s="9">
-        <v>8686938200</v>
+        <v>7004966000</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="E29" s="9">
         <v>1</v>
@@ -5964,16 +6498,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="C30" s="9">
-        <v>7004966000</v>
+        <v>2732996800</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="E30" s="9">
         <v>1</v>
@@ -5981,16 +6515,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="C31" s="9">
-        <v>2732996800</v>
+        <v>3204042600</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="E31" s="9">
         <v>1</v>
@@ -5998,16 +6532,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="C32" s="9">
-        <v>3204042600</v>
+        <v>5784813900</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="E32" s="9">
         <v>1</v>
@@ -6015,16 +6549,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>642</v>
+        <v>313</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>643</v>
+        <v>314</v>
       </c>
       <c r="C33" s="9">
-        <v>5784813900</v>
+        <v>9690076500</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>644</v>
+        <v>152</v>
       </c>
       <c r="E33" s="9">
         <v>1</v>
@@ -6032,16 +6566,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
-        <v>313</v>
+        <v>645</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>314</v>
+        <v>646</v>
       </c>
       <c r="C34" s="9">
-        <v>9690076500</v>
+        <v>948805880</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>152</v>
+        <v>647</v>
       </c>
       <c r="E34" s="9">
         <v>1</v>
@@ -6049,16 +6583,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="C35" s="9">
-        <v>948805880</v>
+        <v>1431115500</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>647</v>
+        <v>627</v>
       </c>
       <c r="E35" s="9">
         <v>1</v>
@@ -6066,16 +6600,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="C36" s="9">
-        <v>1431115500</v>
+        <v>1311547480</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>627</v>
+        <v>652</v>
       </c>
       <c r="E36" s="9">
         <v>1</v>
@@ -6083,16 +6617,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="C37" s="9">
-        <v>1311547480</v>
+        <v>1584898100</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="E37" s="9">
         <v>1</v>
@@ -6100,16 +6634,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="C38" s="9">
-        <v>1584898100</v>
+        <v>1629058200</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="E38" s="9">
         <v>1</v>
@@ -6117,16 +6651,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="C39" s="9">
-        <v>1629058200</v>
+        <v>653763400</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="E39" s="9">
         <v>1</v>
@@ -6134,16 +6668,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
-        <v>659</v>
+        <v>448</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>660</v>
+        <v>449</v>
       </c>
       <c r="C40" s="9">
-        <v>653763400</v>
+        <v>4619774700</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>661</v>
+        <v>450</v>
       </c>
       <c r="E40" s="9">
         <v>1</v>
@@ -6151,16 +6685,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
-        <v>448</v>
+        <v>662</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>449</v>
+        <v>663</v>
       </c>
       <c r="C41" s="9">
-        <v>4619774700</v>
+        <v>4062030000</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>450</v>
+        <v>664</v>
       </c>
       <c r="E41" s="9">
         <v>1</v>
@@ -6168,16 +6702,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="C42" s="9">
-        <v>4062030000</v>
+        <v>2470708800</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="E42" s="9">
         <v>1</v>
@@ -6185,16 +6719,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="C43" s="9">
-        <v>2470708800</v>
+        <v>20263053000</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="E43" s="9">
         <v>1</v>
@@ -6202,16 +6736,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="C44" s="9">
-        <v>20263053000</v>
+        <v>16515344000</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="E44" s="9">
         <v>1</v>
@@ -6219,16 +6753,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="C45" s="9">
-        <v>16515344000</v>
+        <v>4512902400</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>673</v>
+        <v>655</v>
       </c>
       <c r="E45" s="9">
         <v>1</v>
@@ -6236,16 +6770,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="C46" s="9">
-        <v>4512902400</v>
+        <v>18566242000</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>655</v>
+        <v>678</v>
       </c>
       <c r="E46" s="9">
         <v>1</v>
@@ -6253,16 +6787,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="C47" s="9">
-        <v>18566242000</v>
+        <v>18387480000</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="E47" s="9">
         <v>1</v>
@@ -6270,16 +6804,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="C48" s="9">
-        <v>18387480000</v>
+        <v>3483821300</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>681</v>
+        <v>655</v>
       </c>
       <c r="E48" s="9">
         <v>1</v>
@@ -6287,16 +6821,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="C49" s="9">
-        <v>3483821300</v>
+        <v>3179627400</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>655</v>
+        <v>686</v>
       </c>
       <c r="E49" s="9">
         <v>1</v>
@@ -6304,16 +6838,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="C50" s="9">
-        <v>3179627400</v>
+        <v>1529091000</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="E50" s="9">
         <v>1</v>
@@ -6321,16 +6855,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="C51" s="9">
-        <v>1529091000</v>
+        <v>11416550300</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="E51" s="9">
         <v>1</v>
@@ -6338,16 +6872,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="C52" s="9">
-        <v>11416550300</v>
+        <v>5323290400</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="E52" s="9">
         <v>1</v>
@@ -6355,35 +6889,18 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="C53" s="9">
-        <v>5323290400</v>
+        <v>30584329000</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="E53" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="9" t="s">
-        <v>696</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>697</v>
-      </c>
-      <c r="C54" s="9">
-        <v>30584329000</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>698</v>
-      </c>
-      <c r="E54" s="9">
         <v>1</v>
       </c>
     </row>
@@ -6393,17 +6910,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5CAE4A-74D4-46FC-AB35-258346F0AB9F}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="3" width="9.140625" style="9"/>
+    <col min="4" max="4" width="26.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -6425,67 +6944,67 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>375</v>
+        <v>358</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>376</v>
+        <v>273</v>
       </c>
       <c r="C2" s="9">
-        <v>13069483700</v>
+        <v>10225073400</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>377</v>
+        <v>700</v>
       </c>
       <c r="E2" s="9">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>358</v>
+        <v>496</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="C3" s="9">
-        <v>10225073400</v>
+        <v>995415190</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>274</v>
+        <v>701</v>
       </c>
       <c r="E3" s="9">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>496</v>
+        <v>477</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C4" s="9">
-        <v>995415190</v>
+        <v>1758873600</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="E4" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>477</v>
+        <v>129</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>286</v>
+        <v>130</v>
       </c>
       <c r="C5" s="9">
-        <v>1758873600</v>
+        <v>11240573600</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="E5" s="9">
         <v>3</v>
@@ -6493,16 +7012,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>129</v>
+        <v>497</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>130</v>
+        <v>298</v>
       </c>
       <c r="C6" s="9">
-        <v>11240573600</v>
+        <v>924800000</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E6" s="9">
         <v>3</v>
@@ -6510,16 +7029,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>497</v>
+        <v>315</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C7" s="9">
-        <v>924800000</v>
+        <v>43462522000</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="E7" s="9">
         <v>3</v>
@@ -6527,33 +7046,33 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>315</v>
+        <v>349</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="C8" s="9">
-        <v>43462522000</v>
+        <v>8747875200</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>301</v>
+        <v>351</v>
       </c>
       <c r="E8" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>349</v>
+        <v>402</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>350</v>
+        <v>403</v>
       </c>
       <c r="C9" s="9">
-        <v>8747875200</v>
+        <v>2498840000</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>351</v>
+        <v>501</v>
       </c>
       <c r="E9" s="9">
         <v>2</v>
@@ -6561,16 +7080,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>402</v>
+        <v>333</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>403</v>
+        <v>334</v>
       </c>
       <c r="C10" s="9">
-        <v>2498840000</v>
+        <v>2229561900</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="E10" s="9">
         <v>2</v>
@@ -6578,16 +7097,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="C11" s="9">
-        <v>2229561900</v>
+        <v>4301505500</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>502</v>
+        <v>327</v>
       </c>
       <c r="E11" s="9">
         <v>2</v>
@@ -6595,33 +7114,33 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>325</v>
+        <v>503</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>326</v>
+        <v>271</v>
       </c>
       <c r="C12" s="9">
-        <v>4301505500</v>
+        <v>2961655400</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>327</v>
+        <v>272</v>
       </c>
       <c r="E12" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>271</v>
+        <v>146</v>
       </c>
       <c r="C13" s="9">
-        <v>2961655400</v>
+        <v>2300300600</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>272</v>
+        <v>147</v>
       </c>
       <c r="E13" s="9">
         <v>1</v>
@@ -6629,16 +7148,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>146</v>
+        <v>506</v>
       </c>
       <c r="C14" s="9">
-        <v>2300300600</v>
+        <v>3060246800</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>147</v>
+        <v>507</v>
       </c>
       <c r="E14" s="9">
         <v>1</v>
@@ -6646,16 +7165,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="C15" s="9">
-        <v>3060246800</v>
+        <v>3830104200</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="E15" s="9">
         <v>1</v>
@@ -6663,16 +7182,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="C16" s="9">
-        <v>3830104200</v>
+        <v>2395741700</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="E16" s="9">
         <v>1</v>
@@ -6680,16 +7199,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="C17" s="9">
-        <v>2395741700</v>
+        <v>7612651400</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="E17" s="9">
         <v>1</v>
@@ -6697,16 +7216,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="C18" s="9">
-        <v>7612651400</v>
+        <v>3828103800</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="E18" s="9">
         <v>1</v>
@@ -6714,16 +7233,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="C19" s="9">
-        <v>3828103800</v>
+        <v>5121342200</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="E19" s="9">
         <v>1</v>
@@ -6731,16 +7250,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="C20" s="9">
-        <v>5121342200</v>
+        <v>2118877800</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="E20" s="9">
         <v>1</v>
@@ -6748,16 +7267,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="C21" s="9">
-        <v>2118877800</v>
+        <v>6972574900</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="E21" s="9">
         <v>1</v>
@@ -6765,16 +7284,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="C22" s="9">
-        <v>6972574900</v>
+        <v>1390028000</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="E22" s="9">
         <v>1</v>
@@ -6782,16 +7301,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="C23" s="9">
-        <v>1390028000</v>
+        <v>31084242000</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="E23" s="9">
         <v>1</v>
@@ -6799,16 +7318,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="C24" s="9">
-        <v>31084242000</v>
+        <v>9604336400</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="E24" s="9">
         <v>1</v>
@@ -6816,16 +7335,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="C25" s="9">
-        <v>9604336400</v>
+        <v>27497752000</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="E25" s="9">
         <v>1</v>
@@ -6833,16 +7352,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="C26" s="9">
-        <v>27497752000</v>
+        <v>4739788900</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="E26" s="9">
         <v>1</v>
@@ -6850,16 +7369,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
-        <v>541</v>
+        <v>79</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="C27" s="9">
-        <v>4739788900</v>
+        <v>10255441900</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="E27" s="9">
         <v>1</v>
@@ -6867,16 +7386,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
-        <v>79</v>
+        <v>546</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="C28" s="9">
-        <v>10255441900</v>
+        <v>1879035500</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="E28" s="9">
         <v>1</v>
@@ -6884,16 +7403,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="C29" s="9">
-        <v>1879035500</v>
+        <v>1890579600</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="E29" s="9">
         <v>1</v>
@@ -6901,16 +7420,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="C30" s="9">
-        <v>1890579600</v>
+        <v>68390256000</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="E30" s="9">
         <v>1</v>
@@ -6918,16 +7437,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="C31" s="9">
-        <v>68390256000</v>
+        <v>7475561800</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="E31" s="9">
         <v>1</v>
@@ -6935,16 +7454,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="C32" s="9">
-        <v>7475561800</v>
+        <v>58214505000</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="E32" s="9">
         <v>1</v>
@@ -6952,16 +7471,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="C33" s="9">
-        <v>58214505000</v>
+        <v>3276853300</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="E33" s="9">
         <v>1</v>
@@ -6969,16 +7488,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="C34" s="9">
-        <v>3276853300</v>
+        <v>1894585000</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="E34" s="9">
         <v>1</v>
@@ -6986,16 +7505,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="C35" s="9">
-        <v>1894585000</v>
+        <v>2219442500</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="E35" s="9">
         <v>1</v>
@@ -7003,16 +7522,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="C36" s="9">
-        <v>2219442500</v>
+        <v>28848844000</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="E36" s="9">
         <v>1</v>
@@ -7020,16 +7539,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="C37" s="9">
-        <v>28848844000</v>
+        <v>5025589100</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="E37" s="9">
         <v>1</v>
@@ -7037,16 +7556,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="C38" s="9">
-        <v>5025589100</v>
+        <v>2791340700</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="E38" s="9">
         <v>1</v>
@@ -7054,16 +7573,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="C39" s="9">
-        <v>2791340700</v>
+        <v>4506624000</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="E39" s="9">
         <v>1</v>
@@ -7071,35 +7590,18 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="C40" s="9">
-        <v>4506624000</v>
+        <v>39769798000</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="E40" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="9" t="s">
-        <v>582</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>583</v>
-      </c>
-      <c r="C41" s="9">
-        <v>39769798000</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>584</v>
-      </c>
-      <c r="E41" s="9">
         <v>1</v>
       </c>
     </row>
@@ -7110,12 +7612,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8F9ABB-F44C-4F03-BD88-5C978289835A}">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:M80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -7398,7 +7900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>343</v>
       </c>
@@ -7415,7 +7917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>345</v>
       </c>
@@ -7432,7 +7934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>348</v>
       </c>
@@ -7449,7 +7951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>349</v>
       </c>
@@ -7466,7 +7968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>352</v>
       </c>
@@ -7483,7 +7985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>355</v>
       </c>
@@ -7499,8 +8001,11 @@
       <c r="E22" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="M22" s="9" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>358</v>
       </c>
@@ -7517,7 +8022,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>359</v>
       </c>
@@ -7534,7 +8039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>361</v>
       </c>
@@ -7551,7 +8056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
         <v>362</v>
       </c>
@@ -7568,7 +8073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
         <v>365</v>
       </c>
@@ -7585,7 +8090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
         <v>368</v>
       </c>
@@ -7602,7 +8107,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
         <v>369</v>
       </c>
@@ -7619,7 +8124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>372</v>
       </c>
@@ -7636,7 +8141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
         <v>375</v>
       </c>
@@ -7653,7 +8158,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>378</v>
       </c>
@@ -8493,12 +8998,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E403733-B902-45A1-81B8-8A7EFB15CC14}">
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -8525,24 +9030,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="96" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="81" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="81"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
       <c r="O1" s="58"/>
       <c r="P1" s="58"/>
       <c r="Q1" s="58"/>
@@ -8959,678 +9464,6 @@
   <mergeCells count="2">
     <mergeCell ref="E1:N1"/>
     <mergeCell ref="A1:D1"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E0BFF9-F567-4705-9C7E-E21C99F47D06}">
-  <dimension ref="A1:T50"/>
-  <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.35546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1">
-        <v>2020</v>
-      </c>
-      <c r="B1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C1" s="22">
-        <v>44877</v>
-      </c>
-      <c r="D1" s="83" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C2" s="22">
-        <v>44923</v>
-      </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2021</v>
-      </c>
-      <c r="B3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C3" s="22">
-        <v>44566</v>
-      </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B4">
-        <v>3500</v>
-      </c>
-      <c r="C4" s="22">
-        <v>44574</v>
-      </c>
-      <c r="D4" s="95" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" s="83"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C5" s="23">
-        <v>44580</v>
-      </c>
-      <c r="D5" s="95"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C6" s="23">
-        <v>44596</v>
-      </c>
-      <c r="E6" s="95" t="s">
-        <v>98</v>
-      </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C7" s="23">
-        <v>44600</v>
-      </c>
-      <c r="E7" s="95"/>
-      <c r="F7" s="85" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B8">
-        <v>3700</v>
-      </c>
-      <c r="C8" s="23">
-        <v>44616</v>
-      </c>
-      <c r="E8" s="95"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C9" s="23">
-        <v>44628</v>
-      </c>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B10">
-        <v>3300</v>
-      </c>
-      <c r="C10" s="23">
-        <v>44632</v>
-      </c>
-      <c r="G10" s="88" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C11" s="22">
-        <v>44657</v>
-      </c>
-      <c r="D11" s="94" t="s">
-        <v>99</v>
-      </c>
-      <c r="G11" s="88"/>
-      <c r="H11" s="96" t="s">
-        <v>102</v>
-      </c>
-      <c r="I11" s="85" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C12" s="22">
-        <v>44678</v>
-      </c>
-      <c r="D12" s="94"/>
-      <c r="E12" s="96" t="s">
-        <v>100</v>
-      </c>
-      <c r="F12" s="92" t="s">
-        <v>101</v>
-      </c>
-      <c r="H12" s="96"/>
-      <c r="I12" s="85"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C13" s="22">
-        <v>44700</v>
-      </c>
-      <c r="D13" s="94"/>
-      <c r="E13" s="96"/>
-      <c r="F13" s="92"/>
-      <c r="G13" s="93" t="s">
-        <v>106</v>
-      </c>
-      <c r="H13" s="96"/>
-      <c r="I13" s="85"/>
-      <c r="J13" s="85" t="s">
-        <v>104</v>
-      </c>
-      <c r="K13" s="84" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C14" s="22"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="96"/>
-      <c r="F14" s="92"/>
-      <c r="G14" s="93"/>
-      <c r="H14" s="96"/>
-      <c r="I14" s="85"/>
-      <c r="J14" s="85"/>
-      <c r="K14" s="84"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B15">
-        <v>3600</v>
-      </c>
-      <c r="C15" s="22">
-        <v>44720</v>
-      </c>
-      <c r="E15" s="96"/>
-      <c r="F15" s="92"/>
-      <c r="G15" s="93"/>
-      <c r="H15" s="96"/>
-      <c r="J15" s="85"/>
-      <c r="K15" s="84"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C16" s="22">
-        <v>44729</v>
-      </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="93"/>
-      <c r="H16" s="96"/>
-      <c r="J16" s="85"/>
-      <c r="K16" s="84"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C17" s="22">
-        <v>44736</v>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="H17" s="96"/>
-      <c r="K17" s="93" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C18" s="22">
-        <v>44743</v>
-      </c>
-      <c r="G18" s="92" t="s">
-        <v>107</v>
-      </c>
-      <c r="H18" s="96"/>
-      <c r="I18" s="96" t="s">
-        <v>108</v>
-      </c>
-      <c r="J18" s="92" t="s">
-        <v>109</v>
-      </c>
-      <c r="K18" s="93"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B19">
-        <v>3300</v>
-      </c>
-      <c r="G19" s="92"/>
-      <c r="I19" s="96"/>
-      <c r="J19" s="92"/>
-      <c r="K19" s="93"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C20" s="22">
-        <v>44779</v>
-      </c>
-      <c r="G20" s="92"/>
-      <c r="I20" s="96"/>
-      <c r="J20" s="92"/>
-      <c r="K20" s="93"/>
-      <c r="L20" s="96" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C21" s="22"/>
-      <c r="G21" s="92"/>
-      <c r="I21" s="96"/>
-      <c r="J21" s="92"/>
-      <c r="K21" s="93"/>
-      <c r="L21" s="96"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C22" s="22">
-        <v>44805</v>
-      </c>
-      <c r="G22" s="92"/>
-      <c r="I22" s="96"/>
-      <c r="J22" s="92"/>
-      <c r="K22" s="93"/>
-      <c r="L22" s="96"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B23">
-        <v>3700</v>
-      </c>
-      <c r="C23" s="22">
-        <v>44818</v>
-      </c>
-      <c r="G23" s="92"/>
-      <c r="K23" s="93"/>
-      <c r="L23" s="96"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="L24" s="96"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C25" s="22">
-        <v>44863</v>
-      </c>
-      <c r="L25" s="96"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C26" s="22">
-        <v>44866</v>
-      </c>
-      <c r="L26" s="96"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C27" s="22">
-        <v>44884</v>
-      </c>
-      <c r="K27" s="85" t="s">
-        <v>112</v>
-      </c>
-      <c r="L27" s="85" t="s">
-        <v>113</v>
-      </c>
-      <c r="M27" s="84" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>2022</v>
-      </c>
-      <c r="B28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="22">
-        <v>44916</v>
-      </c>
-      <c r="K28" s="85"/>
-      <c r="L28" s="85"/>
-      <c r="M28" s="84"/>
-      <c r="N28" s="85" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B29">
-        <v>3700</v>
-      </c>
-      <c r="C29" s="22">
-        <v>1</v>
-      </c>
-      <c r="L29" s="85"/>
-      <c r="N29" s="85"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C30" s="22">
-        <v>44579</v>
-      </c>
-      <c r="L30" s="85"/>
-      <c r="N30" s="85"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C31" s="22">
-        <v>44599</v>
-      </c>
-      <c r="M31" s="85" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>173</v>
-      </c>
-      <c r="B32" t="s">
-        <v>177</v>
-      </c>
-      <c r="C32" s="22">
-        <v>44622</v>
-      </c>
-      <c r="K32" s="90" t="s">
-        <v>167</v>
-      </c>
-      <c r="M32" s="85"/>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="C33" s="22">
-        <v>44631</v>
-      </c>
-      <c r="K33" s="91"/>
-      <c r="M33" s="85"/>
-      <c r="N33" s="90" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="C34" s="22">
-        <v>44641</v>
-      </c>
-      <c r="K34" s="91"/>
-      <c r="M34" s="85"/>
-      <c r="N34" s="91"/>
-      <c r="O34" s="85" t="s">
-        <v>116</v>
-      </c>
-      <c r="T34" s="82" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>174</v>
-      </c>
-      <c r="B35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35" s="22">
-        <v>44663</v>
-      </c>
-      <c r="N35" s="91"/>
-      <c r="O35" s="85"/>
-      <c r="T35" s="82"/>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B36">
-        <v>2860</v>
-      </c>
-      <c r="C36" s="22">
-        <v>44676</v>
-      </c>
-      <c r="K36" s="85" t="s">
-        <v>119</v>
-      </c>
-      <c r="L36" s="89" t="s">
-        <v>172</v>
-      </c>
-      <c r="M36" s="85" t="s">
-        <v>55</v>
-      </c>
-      <c r="N36" s="85" t="s">
-        <v>117</v>
-      </c>
-      <c r="O36" s="85"/>
-      <c r="T36" s="82"/>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="C37" s="22">
-        <v>44694</v>
-      </c>
-      <c r="I37" s="82" t="s">
-        <v>123</v>
-      </c>
-      <c r="J37" s="86" t="s">
-        <v>170</v>
-      </c>
-      <c r="K37" s="85"/>
-      <c r="L37" s="84"/>
-      <c r="M37" s="85"/>
-      <c r="N37" s="85"/>
-      <c r="O37" s="85"/>
-      <c r="P37" s="84" t="s">
-        <v>168</v>
-      </c>
-      <c r="R37" s="87" t="s">
-        <v>166</v>
-      </c>
-      <c r="S37" s="85" t="s">
-        <v>120</v>
-      </c>
-      <c r="T37" s="82"/>
-    </row>
-    <row r="38" spans="1:20" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>175</v>
-      </c>
-      <c r="B38" t="s">
-        <v>178</v>
-      </c>
-      <c r="C38" s="22">
-        <v>44702</v>
-      </c>
-      <c r="D38" s="83" t="s">
-        <v>122</v>
-      </c>
-      <c r="I38" s="82"/>
-      <c r="J38" s="83"/>
-      <c r="K38" s="85"/>
-      <c r="L38" s="85" t="s">
-        <v>118</v>
-      </c>
-      <c r="M38" s="85"/>
-      <c r="N38" s="85"/>
-      <c r="O38" s="84" t="s">
-        <v>121</v>
-      </c>
-      <c r="P38" s="84"/>
-      <c r="Q38" s="84" t="s">
-        <v>169</v>
-      </c>
-      <c r="R38" s="88"/>
-      <c r="S38" s="85"/>
-      <c r="T38" s="82"/>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="C39" s="22">
-        <v>44721</v>
-      </c>
-      <c r="D39" s="83"/>
-      <c r="E39" s="82" t="s">
-        <v>145</v>
-      </c>
-      <c r="G39" s="84" t="s">
-        <v>124</v>
-      </c>
-      <c r="I39" s="82"/>
-      <c r="J39" s="83"/>
-      <c r="L39" s="85"/>
-      <c r="O39" s="84"/>
-      <c r="P39" s="84"/>
-      <c r="Q39" s="84"/>
-      <c r="R39" s="88"/>
-      <c r="S39" s="85"/>
-      <c r="T39" s="82"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="C40" s="22">
-        <v>44725</v>
-      </c>
-      <c r="D40" s="83"/>
-      <c r="E40" s="82"/>
-      <c r="G40" s="84"/>
-      <c r="H40" s="85" t="s">
-        <v>73</v>
-      </c>
-      <c r="I40" s="82"/>
-      <c r="J40" s="83"/>
-      <c r="L40" s="33"/>
-      <c r="O40" s="84"/>
-      <c r="P40" s="34"/>
-      <c r="Q40" s="34"/>
-      <c r="R40" s="88"/>
-      <c r="S40" s="85"/>
-      <c r="T40" s="35"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A41" s="42" t="s">
-        <v>176</v>
-      </c>
-      <c r="B41">
-        <v>3316</v>
-      </c>
-      <c r="C41" s="22">
-        <v>44729</v>
-      </c>
-      <c r="D41" s="83"/>
-      <c r="E41" s="82"/>
-      <c r="G41" s="84"/>
-      <c r="H41" s="85"/>
-      <c r="I41" s="82"/>
-      <c r="J41" s="83"/>
-      <c r="O41" s="84"/>
-      <c r="R41" s="88"/>
-      <c r="S41" s="85"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="D42" s="83"/>
-      <c r="E42" s="82"/>
-      <c r="G42" s="84"/>
-      <c r="H42" s="85"/>
-      <c r="I42" s="82"/>
-      <c r="J42" s="83"/>
-      <c r="O42" s="84"/>
-      <c r="R42" s="88"/>
-      <c r="S42" s="85"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A43" s="43" t="s">
-        <v>179</v>
-      </c>
-      <c r="D43" s="83"/>
-      <c r="E43" s="82"/>
-      <c r="G43" s="84"/>
-      <c r="H43" s="85"/>
-      <c r="I43" s="82"/>
-      <c r="J43" s="83"/>
-      <c r="O43" s="84"/>
-      <c r="R43" s="88"/>
-      <c r="S43" s="85"/>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="D44" s="83"/>
-      <c r="E44" s="82"/>
-      <c r="G44" s="84"/>
-      <c r="H44" s="85"/>
-      <c r="I44" s="82"/>
-      <c r="J44" s="83"/>
-      <c r="O44" s="84"/>
-      <c r="R44" s="88"/>
-      <c r="S44" s="85"/>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="D45" s="83"/>
-      <c r="E45" s="82"/>
-      <c r="G45" s="84"/>
-      <c r="H45" s="85"/>
-      <c r="I45" s="82"/>
-      <c r="J45" s="83"/>
-      <c r="R45" s="88"/>
-      <c r="S45" s="85"/>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="D46" s="83"/>
-      <c r="E46" s="82"/>
-      <c r="G46" s="84"/>
-      <c r="H46" s="85"/>
-      <c r="I46" s="82"/>
-      <c r="J46" s="83"/>
-      <c r="R46" s="88"/>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="E47" s="82"/>
-      <c r="H47" s="85"/>
-      <c r="I47" s="82"/>
-      <c r="J47" s="83"/>
-      <c r="R47" s="88"/>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="E48" s="82"/>
-      <c r="H48" s="85"/>
-    </row>
-    <row r="49" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E49" s="82"/>
-      <c r="H49" s="85"/>
-    </row>
-    <row r="50" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E50" s="82"/>
-    </row>
-  </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="H11:H18"/>
-    <mergeCell ref="I18:I22"/>
-    <mergeCell ref="J18:J22"/>
-    <mergeCell ref="K17:K23"/>
-    <mergeCell ref="J13:J16"/>
-    <mergeCell ref="K13:K16"/>
-    <mergeCell ref="I11:I14"/>
-    <mergeCell ref="L20:L26"/>
-    <mergeCell ref="M31:M34"/>
-    <mergeCell ref="K27:K28"/>
-    <mergeCell ref="L27:L30"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G18:G23"/>
-    <mergeCell ref="G13:G16"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="N33:N35"/>
-    <mergeCell ref="K32:K34"/>
-    <mergeCell ref="T34:T39"/>
-    <mergeCell ref="N28:N30"/>
-    <mergeCell ref="E39:E50"/>
-    <mergeCell ref="D38:D46"/>
-    <mergeCell ref="I37:I47"/>
-    <mergeCell ref="G39:G46"/>
-    <mergeCell ref="S37:S45"/>
-    <mergeCell ref="K36:K38"/>
-    <mergeCell ref="P37:P39"/>
-    <mergeCell ref="H40:H49"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="O38:O44"/>
-    <mergeCell ref="J37:J47"/>
-    <mergeCell ref="R37:R47"/>
-    <mergeCell ref="Q38:Q39"/>
-    <mergeCell ref="M36:M38"/>
-    <mergeCell ref="O34:O37"/>
-    <mergeCell ref="N36:N38"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>